<commit_message>
10: Correct AC Extension Cable description
The cable is linked correctly but, as described in the Motherboard Assembly Guide, it is intended to be 6 feet.
</commit_message>
<xml_diff>
--- a/BOM food computer.xlsx
+++ b/BOM food computer.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camille\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\Desktop\git\gro-hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,7 @@
     <sheet name="Kit" sheetId="3" r:id="rId3"/>
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -253,9 +252,6 @@
     <t>Leviton T5320-W 15 Amp, 125 Volt, Tamper Resistant, Duplex Receptacle, Residential Grade, Grounding, White</t>
   </si>
   <si>
-    <t>C2G / Cables To Go 03137 18 AWG Outlet Saver Power Extension Cord for NEMA 5-15P to NEMA 5-15R, Black (1 Foot/0.30 Meters)</t>
-  </si>
-  <si>
     <t>LIGHTS</t>
   </si>
   <si>
@@ -584,12 +580,15 @@
   </si>
   <si>
     <t>measure out fertilizers, yeast, and sugar</t>
+  </si>
+  <si>
+    <t>C2G / Cables To Go 03137 18 AWG Outlet Saver Power Extension Cord for NEMA 5-15P to NEMA 5-15R, Black (6 Foot/1.82 Meters)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -904,6 +903,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -939,6 +955,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1093,21 +1126,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1137,7 +1170,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CyberPower-CSB606-Protector-6-Outlets-Joules/dp/B00FLTTGYG/ref=pd_sim_23_1?ie=UTF8&amp;refRID=163NC2W6A2KW7EF2RB9B","Power Strip")</f>
         <v>Power Strip</v>
@@ -1159,7 +1192,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Switching-Power-Supply-Strip-Light/dp/B007MWNF5Q/ref=pd_sim_60_6?ie=UTF8&amp;refRID=0WA6QTYVKRWRGRG1ZKN2A","Main Power Supply")</f>
         <v>Main Power Supply</v>
@@ -1181,7 +1214,7 @@
         <v>24.96</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
@@ -1203,7 +1236,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1213,7 +1246,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CanaKit-Raspberry-Power-Supply-Listed/dp/B00MARDJZ4/ref=sr_1_2?ie=UTF8&amp;qid=1439988175&amp;sr=8-2&amp;keywords=raspberry+pi+2+power+supply","Raspberry Pi Power Supply")</f>
         <v>Raspberry Pi Power Supply</v>
@@ -1235,7 +1268,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Ximico-Arduino-Cable-Atmega2560-16au-Compatible/dp/B00KG3SBE8/ref=sr_1_2?s=pc&amp;ie=UTF8&amp;qid=1439935660&amp;sr=1-2&amp;keywords=arduino+mega","Arduino Mega 2560")</f>
         <v>Arduino Mega 2560</v>
@@ -1257,7 +1290,7 @@
         <v>14.19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Raspberry-Pi-Model-Desktop-Linux/dp/B00T2U7R7I","Raspberry Pi 2 Model B")</f>
         <v>Raspberry Pi 2 Model B</v>
@@ -1279,7 +1312,7 @@
         <v>41.87</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Kingston-microSDHC-Memory-SDC4-8GBET/dp/B00200K1TS/ref=sr_1_8?s=pc&amp;ie=UTF8&amp;qid=1439988385&amp;sr=1-8&amp;keywords=micro+SD","Micro SD Card")</f>
         <v>Micro SD Card</v>
@@ -1301,7 +1334,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EUHRLF6/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=A1DCPNQKKEISZB","Ethernet cable")</f>
         <v>Ethernet cable</v>
@@ -1320,7 +1353,7 @@
         <v>5.99</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Gikfun-Protoshield-Prototype-Shield-Arduino/dp/B00Q9YBQ04/ref=sr_1_6?s=pc&amp;ie=UTF8&amp;qid=1439935499&amp;sr=1-6&amp;keywords=protoshield","Arduino Mega Protoshield")</f>
         <v>Arduino Mega Protoshield</v>
@@ -1342,7 +1375,7 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Base-Shield-V2-p-1378.html","Grove Base Shield")</f>
         <v>Grove Base Shield</v>
@@ -1364,7 +1397,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
         <f>HYPERLINK("https://www.adafruit.com/products/2097","Touchscreen Display")</f>
         <v>Touchscreen Display</v>
@@ -1386,7 +1419,7 @@
         <v>44.95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/ribbon-cable-Raspberry-stackable-header/dp/B00G84WNA2/ref=sr_1_1?ie=UTF8&amp;qid=1440708449&amp;sr=8-1&amp;keywords=raspberry+pi+cable","GPIO Cable ")</f>
         <v xml:space="preserve">GPIO Cable </v>
@@ -1408,7 +1441,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>71</v>
       </c>
@@ -1418,7 +1451,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/JBtek-Channel-Module-Arduino-Raspberry/dp/B00KTEN3TM/ref=sr_1_1?s=pc&amp;ie=UTF8&amp;qid=1439935182&amp;sr=1-1&amp;keywords=4+Channel+Relay","4-Channel Relay")</f>
         <v>4-Channel Relay</v>
@@ -1440,7 +1473,7 @@
         <v>13.96</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/52171-4E-Pre-Galvanized-Eccentric-Knockouts/dp/B000HEFCKC/ref=pd_bxgy_60_text_y","AC Relay Box Back Receptacle")</f>
         <v>AC Relay Box Back Receptacle</v>
@@ -1462,7 +1495,7 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/RS8-Outlet-Surface-Square-Galvanized/dp/B000HEIU9W/ref=pd_sim_60_23?ie=UTF8&amp;refRID=0C95J370DWVEWW0H1MG8","AC Relay Box Front Panel")</f>
         <v>AC Relay Box Front Panel</v>
@@ -1484,7 +1517,7 @@
         <v>4.92</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Leviton-T5320-W-Resistant-Receptacle-Residential/dp/B0015R9M2Y/ref=pd_bxgy_60_img_z","AC Plug")</f>
         <v>AC Plug</v>
@@ -1506,7 +1539,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
@@ -1515,22 +1548,22 @@
         <v>16</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>76</v>
+        <v>186</v>
       </c>
       <c r="D21" s="8">
         <v>1</v>
       </c>
       <c r="E21" s="8">
-        <v>4.99</v>
+        <v>5.7</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="3"/>
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1538,7 +1571,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Triangle-Bulbs-T93007-Waterproof-Flexible/dp/B005EHHLD8/ref=sr_1_1?ie=UTF8&amp;qid=1443799060&amp;sr=8-1&amp;keywords=waterproof+led+strip","White LED Strip")</f>
         <v>White LED Strip</v>
@@ -1547,7 +1580,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="8">
         <v>2</v>
@@ -1560,7 +1593,7 @@
         <v>19.98</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Erligpowht-Indoor-Garden-Plant-Hanging/dp/B00S2DPYQM/ref=sr_1_fkmr2_2?ie=UTF8&amp;qid=1443799150&amp;sr=8-2-fkmr2&amp;keywords=grow+led+panel+erwl","Grow LED Panel")</f>
         <v>Grow LED Panel</v>
@@ -1569,7 +1602,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D24" s="8">
         <v>2</v>
@@ -1582,9 +1615,9 @@
         <v>75.98</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1592,7 +1625,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B003XDTWN2/ref=sr_ph?&amp;ie=UTF8&amp;qid=1440085101&amp;sr=1&amp;keywords=heater","Heater")</f>
         <v>Heater</v>
@@ -1601,7 +1634,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="15">
         <v>1</v>
@@ -1614,7 +1647,7 @@
         <v>15.99</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Acoustic-Audio-Tek%C2%A8Portable-Humidifier-travel--White/dp/B00RM5Z44S/ref=sr_1_4?s=home-garden&amp;ie=UTF8&amp;qid=1440427700&amp;sr=1-4&amp;keywords=bottle+cap+humidifier","Humidifier")</f>
         <v>Humidifier</v>
@@ -1623,7 +1656,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="15">
         <v>1</v>
@@ -1636,7 +1669,7 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B00WJW3NM4/ref=twister_B00WJW3M3Y?_encoding=UTF8&amp;psc=1","USB Wall Adapter")</f>
         <v>USB Wall Adapter</v>
@@ -1645,7 +1678,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="8">
         <v>1</v>
@@ -1658,7 +1691,7 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Bgears-b-Blaster-120mm-Bearing-Extreme/dp/B0043GKY1W/ref=sr_1_1?ie=UTF8&amp;qid=1440020490&amp;sr=8-1&amp;keywords=bgears+120mm","Circulation/Vent Fans")</f>
         <v>Circulation/Vent Fans</v>
@@ -1667,7 +1700,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" s="15">
         <v>2</v>
@@ -1680,7 +1713,7 @@
         <v>25.86</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Tjernlund-1519003-Wire-Fan-Guard/dp/B008RMKFTO/ref=sr_1_2?ie=UTF8&amp;qid=1440019946&amp;sr=8-2&amp;keywords=fan+guard","Fan Guards")</f>
         <v>Fan Guards</v>
@@ -1689,7 +1722,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30" s="15">
         <v>2</v>
@@ -1702,7 +1735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Dundas-Jafine-LC4WZW-ProVent-4-Inches/dp/B0016487CC/ref=sr_1_3?ie=UTF8&amp;qid=1440020385&amp;sr=8-3&amp;keywords=Louvered+Vent+Cap","Fan Louvres")</f>
         <v>Fan Louvres</v>
@@ -1711,7 +1744,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="15">
         <v>2</v>
@@ -1724,9 +1757,9 @@
         <v>13.68</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1734,16 +1767,16 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="str">
         <f>HYPERLINK("http://www.co2meter.com/products/cozir-0-2-co2-sensor","CO2 Sensor")</f>
         <v>CO2 Sensor</v>
       </c>
       <c r="B33" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>89</v>
       </c>
       <c r="D33" s="15">
         <v>1</v>
@@ -1756,7 +1789,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-TemperatureHumidity-Sensor-Pro-p-838.html","Air Temperature and Humidity Sensor")</f>
         <v>Air Temperature and Humidity Sensor</v>
@@ -1765,7 +1798,7 @@
         <v>66</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="15">
         <v>1</v>
@@ -1778,7 +1811,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-Digital-Light-Sensor-p-1281.html","Light Intensity Sensor")</f>
         <v>Light Intensity Sensor</v>
@@ -1787,7 +1820,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" s="15">
         <v>1</v>
@@ -1800,7 +1833,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00YCDHQ8K?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o06_s00","Webcam")</f>
         <v>Webcam</v>
@@ -1809,7 +1842,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36" s="8">
         <v>1</v>
@@ -1822,9 +1855,9 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1832,7 +1865,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009SUF08?keywords=reed%20switch&amp;qid=1443805349&amp;ref_=sr_1_1&amp;sr=8-1","Magnetic Switch")</f>
         <v>Magnetic Switch</v>
@@ -1841,7 +1874,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D38" s="8">
         <v>1</v>
@@ -1854,16 +1887,16 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Micro-Limit-Switch-Roller-Action/dp/B00E0JOTV8/ref=sr_1_1?s=lamps-light&amp;ie=UTF8&amp;qid=1443805532&amp;sr=1-1&amp;keywords=limit+switch","Limit Switch")</f>
         <v>Limit Switch</v>
       </c>
       <c r="B39" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="D39" s="8">
         <v>1</v>
@@ -1876,9 +1909,9 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1886,7 +1919,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009YJ4N6?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Air Pump")</f>
         <v>Air Pump</v>
@@ -1895,7 +1928,7 @@
         <v>16</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41" s="15">
         <v>1</v>
@@ -1908,7 +1941,7 @@
         <v>9.3800000000000008</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Jardin-Aquarium-Ceramic-Diffusers-Diameter/dp/B0050HJ7Q6/ref=pd_bxgy_199_img_z","Air Stone")</f>
         <v>Air Stone</v>
@@ -1917,7 +1950,7 @@
         <v>16</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D42" s="15">
         <v>1</v>
@@ -1930,7 +1963,7 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Standard-Airline-Tubing-Accessories-25-Feet/dp/B0002563MW/ref=pd_bxgy_199_img_y","Air Pump Tubing")</f>
         <v>Air Pump Tubing</v>
@@ -1939,7 +1972,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" s="15">
         <v>1</v>
@@ -1952,16 +1985,16 @@
         <v>4.04</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EWENMAU?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_2&amp;smid=A14L9DIA3NK9B0","Aquarium Pump")</f>
         <v>Aquarium Pump</v>
       </c>
       <c r="B44" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>101</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>102</v>
       </c>
       <c r="D44" s="8">
         <v>1</v>
@@ -1974,16 +2007,16 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0079QUTSQ?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Pump Tubing")</f>
         <v>Pump Tubing</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="8">
         <v>1</v>
@@ -1996,9 +2029,9 @@
         <v>14.39</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2006,16 +2039,16 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1123&amp;search=DFR0300#.VdTDoFNViko","Water Temperature and EC Sensor")</f>
         <v>Water Temperature and EC Sensor</v>
       </c>
       <c r="B47" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>105</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>106</v>
       </c>
       <c r="D47" s="15">
         <v>1</v>
@@ -2028,16 +2061,16 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1025#.Vg60SBNViko","pH Sensor")</f>
         <v>pH Sensor</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D48" s="15">
         <v>1</v>
@@ -2050,9 +2083,9 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2060,7 +2093,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00BL63ZU4?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o01_s00","Cable Management Box")</f>
         <v>Cable Management Box</v>
@@ -2069,7 +2102,7 @@
         <v>16</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D50" s="8">
         <v>1</v>
@@ -2082,7 +2115,7 @@
         <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
@@ -2090,9 +2123,9 @@
       <c r="E51" s="19"/>
       <c r="F51" s="19"/>
     </row>
-    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2100,7 +2133,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="str">
         <f>HYPERLINK("C2G / Cables To Go 53408 18 AWG Outlet Saver Power Extension Cord for NEMA 5-15P to NEMA 5-15R, Black (12 Feet/3.65 Meters)","Sacrificial AC Extension Cable for high gauge wire")</f>
         <v>Sacrificial AC Extension Cable for high gauge wire</v>
@@ -2109,7 +2142,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" s="8">
         <v>1</v>
@@ -2122,7 +2155,7 @@
         <v>10.93</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Wago-222-412-222-413-Lever-Nut-Assortment/dp/B00U4520JK/ref=sr_1_1?ie=UTF8&amp;qid=1443798480&amp;sr=8-1&amp;keywords=wago+lever+nut+assortment","Wago Lever Nut Assortment")</f>
         <v>Wago Lever Nut Assortment</v>
@@ -2131,7 +2164,7 @@
         <v>16</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54" s="8">
         <v>1</v>
@@ -2144,7 +2177,7 @@
         <v>39.99</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Vktech-150pcs-Shrink-Tubing-Sleeving/dp/B00EXLPLTW/ref=sr_1_2?ie=UTF8&amp;qid=1440019080&amp;sr=8-2&amp;keywords=vktech+heat+shrink","Heat Shrink Tubing")</f>
         <v>Heat Shrink Tubing</v>
@@ -2153,7 +2186,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="15">
         <v>1</v>
@@ -2166,7 +2199,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-c-98_106_57/?ref=crumb","Grove Cables")</f>
         <v>Grove Cables</v>
@@ -2175,32 +2208,32 @@
         <v>66</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="19"/>
       <c r="F56" s="19"/>
     </row>
-    <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19"/>
       <c r="F57" s="19"/>
     </row>
-    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/3M-Scotch-1-in-x-12-5-yds-Indoor-Outdoor-Mounting-Tape-411-LONG-DC/100153200","Foam mounting tape")</f>
         <v>Foam mounting tape</v>
       </c>
       <c r="B58" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>117</v>
       </c>
       <c r="D58" s="8">
         <v>1</v>
@@ -2213,16 +2246,16 @@
         <v>15.97</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="str">
         <f>HYPERLINK("http://www.amazon.com/3M-Electrical-75-Inch-66-Foot-0085-Inch/dp/B00004WCCP/ref=sr_1_1?s=industrial&amp;ie=UTF8&amp;qid=1443807012&amp;sr=1-1&amp;keywords=electrical+tape","Electrical Tape")</f>
         <v>Electrical Tape</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" s="8">
         <v>1</v>
@@ -2235,16 +2268,16 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="str">
         <f>HYPERLINK("http://www.digikey.com/product-search/en?KeyWords=377-2132-ND&amp;WT.z_header=search_go","Air Exchange Box")</f>
         <v>Air Exchange Box</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="D60" s="8">
         <v>1</v>
@@ -2257,16 +2290,16 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-6-x-1-2-in-Stainless-Steel-Pan-Head-Phillips-Sheet-Metal-Screw-50-per-Pack-800162/204275035","Short Screws")</f>
         <v>Short Screws</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D61" s="8">
         <v>1</v>
@@ -2279,16 +2312,16 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-8-x-2-in-Zinc-Plated-Pan-Head-Phillips-Drive-Sheet-Metal-Screw-50-Piece-801632/204275094","Long Screws")</f>
         <v>Long Screws</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D62" s="8">
         <v>1</v>
@@ -2301,9 +2334,9 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2313,15 +2346,16 @@
       </c>
       <c r="E63" s="27">
         <f>SUM(F2:F62)</f>
-        <v>840.56</v>
+        <v>841.27</v>
       </c>
       <c r="F63" s="26">
         <f>SUM(F2:F62)</f>
-        <v>840.56</v>
+        <v>841.27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2331,18 +2365,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -2368,7 +2402,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2393,7 +2427,7 @@
       </c>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2418,7 +2452,7 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2443,7 +2477,7 @@
       </c>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2468,7 +2502,7 @@
       </c>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2493,7 +2527,7 @@
       </c>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2518,7 +2552,7 @@
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2543,7 +2577,7 @@
       </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2568,7 +2602,7 @@
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2593,7 +2627,7 @@
       </c>
       <c r="H10" s="17"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2618,7 +2652,7 @@
       </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2643,7 +2677,7 @@
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2668,7 +2702,7 @@
       </c>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2693,7 +2727,7 @@
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2718,7 +2752,7 @@
       </c>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2745,7 +2779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2770,7 +2804,7 @@
       </c>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2795,7 +2829,7 @@
       </c>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2820,7 +2854,7 @@
       </c>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2845,7 +2879,7 @@
       </c>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2870,7 +2904,7 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -2885,7 +2919,7 @@
       </c>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -2895,7 +2929,7 @@
       <c r="G23" s="21"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -2905,7 +2939,7 @@
       <c r="G24" s="21"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -2915,35 +2949,35 @@
       <c r="G25" s="21"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
     </row>
-    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
     </row>
-    <row r="33" spans="6:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
     </row>
@@ -2980,19 +3014,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -3012,20 +3046,20 @@
         <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28">
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>126</v>
       </c>
       <c r="D2" s="28">
         <v>1</v>
@@ -3046,15 +3080,15 @@
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>127</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>128</v>
       </c>
       <c r="D3" s="32">
         <v>1</v>
@@ -3064,7 +3098,7 @@
         <v>JRPeters</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" s="28">
         <v>29.99</v>
@@ -3075,15 +3109,15 @@
       <c r="K3" s="31"/>
       <c r="L3" s="31"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="32">
         <v>1</v>
@@ -3093,7 +3127,7 @@
         <v>JRPeters</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="28">
         <v>29.99</v>
@@ -3104,15 +3138,15 @@
       <c r="K4" s="31"/>
       <c r="L4" s="31"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>132</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>133</v>
       </c>
       <c r="D5" s="32">
         <v>1</v>
@@ -3122,7 +3156,7 @@
         <v>Amazon Prime</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G5" s="32">
         <v>9.99</v>
@@ -3133,15 +3167,15 @@
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="32">
         <v>1</v>
@@ -3162,15 +3196,15 @@
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>142</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>143</v>
       </c>
       <c r="D7" s="32">
         <v>10</v>
@@ -3191,15 +3225,15 @@
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D8" s="32">
         <v>1</v>
@@ -3220,15 +3254,15 @@
       <c r="K8" s="31"/>
       <c r="L8" s="31"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="35" t="s">
         <v>173</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>174</v>
       </c>
       <c r="D9" s="32">
         <v>1</v>
@@ -3249,15 +3283,15 @@
       <c r="K9" s="31"/>
       <c r="L9" s="31"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28">
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="35" t="s">
         <v>175</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>176</v>
       </c>
       <c r="D10" s="32">
         <v>6</v>
@@ -3278,25 +3312,25 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="D11" s="32" t="s">
         <v>178</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>179</v>
       </c>
       <c r="E11" s="33" t="str">
         <f>HYPERLINK("http://www.amazon.com/Watts-SVGE10-Pre-Cut-Diameter-10-Foot/dp/B000HE5DUG/ref=pd_sim_60_4?ie=UTF8&amp;refRID=09WC8C60A2AF6W59DZM7&amp;dpID=41P%2BeRnccFL&amp;dpSrc=sims&amp;preST=_AC_UL160_SR160%2C160_","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G11" s="32">
         <v>7.31</v>
@@ -3307,15 +3341,15 @@
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="35" t="s">
         <v>181</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>182</v>
       </c>
       <c r="D12" s="32">
         <v>1</v>
@@ -3336,15 +3370,15 @@
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>12</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>183</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>184</v>
       </c>
       <c r="D13" s="32">
         <v>1</v>
@@ -3365,15 +3399,15 @@
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36">
         <v>13</v>
       </c>
       <c r="B14" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="37" t="s">
         <v>185</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>186</v>
       </c>
       <c r="D14" s="36">
         <v>1</v>
@@ -3394,7 +3428,7 @@
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="39"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -3413,7 +3447,7 @@
       <c r="K15" s="39"/>
       <c r="L15" s="39"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -3427,7 +3461,7 @@
       <c r="K16" s="39"/>
       <c r="L16" s="39"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -3441,7 +3475,7 @@
       <c r="K17" s="39"/>
       <c r="L17" s="39"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -3455,7 +3489,7 @@
       <c r="K18" s="39"/>
       <c r="L18" s="39"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
@@ -3497,252 +3531,252 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="D1" s="42"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="42"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="B2" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="C2" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="D2" s="42"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="42"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
-        <v>139</v>
-      </c>
       <c r="B3" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="D3" s="42"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="42"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="B4" s="43" t="s">
         <v>146</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>147</v>
       </c>
       <c r="C4" s="45"/>
       <c r="D4" s="42"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>148</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>149</v>
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="42"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="43" t="s">
         <v>150</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>151</v>
       </c>
       <c r="C6" s="45"/>
       <c r="D6" s="42"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
       <c r="D7" s="42"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="42"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="42"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="42"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
       <c r="D11" s="42"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
       <c r="D12" s="42"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="42"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
       <c r="D14" s="42"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" s="45"/>
       <c r="C15" s="45"/>
       <c r="D15" s="42"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
       <c r="D16" s="42"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
       <c r="D17" s="42"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
       <c r="D18" s="42"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
       <c r="D19" s="42"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
       <c r="D20" s="42"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
       <c r="D21" s="42"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
       <c r="D22" s="42"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
       <c r="D23" s="42"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
       <c r="D24" s="42"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B25" s="45"/>
       <c r="C25" s="45"/>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>

</xml_diff>